<commit_message>
using human gtf from ucsc (ensembl genes)
</commit_message>
<xml_diff>
--- a/analyses/maskGenomes/pathsToMaskingFiles.xlsx
+++ b/analyses/maskGenomes/pathsToMaskingFiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annabelbeichman/Documents/UW/DNAShapeProject/scripts/DNA_Shape_Project/analyses/maskGenomes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC0FD02-9A96-2345-AC61-FF5D20E2F4CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244BAE8B-EE5F-B243-AC46-BE5912DDF2C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="520" windowWidth="36860" windowHeight="20060" xr2:uid="{69AA28EC-8F56-B44C-B7AC-A26DE8F0EC11}"/>
   </bookViews>
@@ -148,9 +148,6 @@
     <t xml:space="preserve">/net/harris/vol1/home/beichman/reference_genomes/homo_sapiens_ancestor_GRCh38/allChrs.fai  </t>
   </si>
   <si>
-    <t>/net/harris/vol1/home/beichman/reference_genomes/human_GRCh38_annotation/GRCh38_latest_genomic.gff.gz</t>
-  </si>
-  <si>
     <t>/net/harris/vol1/home/beichman/reference_genomes/human_GRCh38_annotation/repeatmask.sorted.bed</t>
   </si>
   <si>
@@ -239,6 +236,9 @@
   </si>
   <si>
     <t>/net/harris/vol1/home/beichman/reference_genomes/mouse/mm10_aka_mm38/mm10.fa.ADDEDCHRTONUMBERS.fai</t>
+  </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/reference_genomes/human_GRCh38_annotation/hg38.ensGene.gtf.gz</t>
   </si>
 </sst>
 </file>
@@ -619,7 +619,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -629,7 +629,7 @@
     <col min="4" max="4" width="32.83203125" customWidth="1"/>
     <col min="5" max="5" width="49" customWidth="1"/>
     <col min="6" max="6" width="49.83203125" customWidth="1"/>
-    <col min="7" max="7" width="29.5" customWidth="1"/>
+    <col min="7" max="7" width="116.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -672,19 +672,19 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
         <v>40</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>41</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>42</v>
       </c>
-      <c r="F2" t="s">
-        <v>43</v>
-      </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H2" t="s">
         <v>7</v>
@@ -701,16 +701,16 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
         <v>47</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>48</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>49</v>
-      </c>
-      <c r="F3" t="s">
-        <v>50</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>11</v>
@@ -730,19 +730,19 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" t="s">
         <v>52</v>
-      </c>
-      <c r="F4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G4" t="s">
-        <v>53</v>
       </c>
       <c r="H4" t="s">
         <v>33</v>
@@ -768,13 +768,13 @@
         <v>36</v>
       </c>
       <c r="E5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" t="s">
         <v>37</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>38</v>
-      </c>
-      <c r="G5" t="s">
-        <v>39</v>
       </c>
       <c r="H5" t="s">
         <v>33</v>
@@ -791,13 +791,13 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
         <v>54</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>55</v>
-      </c>
-      <c r="E6" t="s">
-        <v>56</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>32</v>
@@ -817,19 +817,19 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" t="s">
         <v>57</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>58</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>59</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>60</v>
-      </c>
-      <c r="G7" t="s">
-        <v>61</v>
       </c>
       <c r="H7" t="s">
         <v>33</v>
@@ -848,10 +848,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding script from https://github.com/hdashnow/TandemRepeatFinder_scripts to convert trf to bed
</commit_message>
<xml_diff>
--- a/analyses/maskGenomes/pathsToMaskingFiles.xlsx
+++ b/analyses/maskGenomes/pathsToMaskingFiles.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annabelbeichman/Documents/UW/DNAShapeProject/scripts/DNA_Shape_Project/analyses/maskGenomes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244BAE8B-EE5F-B243-AC46-BE5912DDF2C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409C8965-588A-9C46-90BF-B977DE9BD97A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="520" windowWidth="36860" windowHeight="20060" xr2:uid="{69AA28EC-8F56-B44C-B7AC-A26DE8F0EC11}"/>
+    <workbookView xWindow="500" yWindow="520" windowWidth="36860" windowHeight="20060" activeTab="1" xr2:uid="{69AA28EC-8F56-B44C-B7AC-A26DE8F0EC11}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="GenomeFiles" sheetId="1" r:id="rId1"/>
+    <sheet name="PreprocessingNotes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="100">
   <si>
     <t>Species</t>
   </si>
@@ -79,6 +80,9 @@
     <t>/net/harris/vol1/home/beichman/reference_genomes/mouse/mm10_aka_mm38</t>
   </si>
   <si>
+    <t>NA</t>
+  </si>
+  <si>
     <t>Human</t>
   </si>
   <si>
@@ -143,9 +147,6 @@
   </si>
   <si>
     <t>not using ^^</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/net/harris/vol1/home/beichman/reference_genomes/homo_sapiens_ancestor_GRCh38/allChrs.fai  </t>
   </si>
   <si>
     <t>/net/harris/vol1/home/beichman/reference_genomes/human_GRCh38_annotation/repeatmask.sorted.bed</t>
@@ -240,12 +241,120 @@
   <si>
     <t>/net/harris/vol1/home/beichman/reference_genomes/human_GRCh38_annotation/hg38.ensGene.gtf.gz</t>
   </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/reference_genomes/human_GRCh38_annotation/hg38.fa.gz.fai</t>
+  </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/reference_genomes/brown_bear/RepeatMaskerOutput_parallel/brown_bear.fasta.RepeatMasker.output.sorted.bed</t>
+  </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/reference_genomes/unifiedBedMasksForAllGenomes/minke_whale_GCF_000493695.1_BalAcu1.0</t>
+  </si>
+  <si>
+    <t>exon10kb+repmask+trf unified bed USE THIS</t>
+  </si>
+  <si>
+    <t>minke_whale_GCF_000493695.1_BalAcu1.0.exon10kb.repmask.trf.NEGATIVEMASK.merged.USETHIS.bed</t>
+  </si>
+  <si>
+    <t>exon10kb only</t>
+  </si>
+  <si>
+    <t>minke_whale_GCF_000493695.1_BalAcu1.0.exonMask.fromGFF_or_GTF.plusminus10kb.0based.sorted.merged.bed</t>
+  </si>
+  <si>
+    <t>rep mask only</t>
+  </si>
+  <si>
+    <t>minke_whale_GCF_000493695.1_BalAcu1.0.repeatMasker.0based.sorted.merged.bed</t>
+  </si>
+  <si>
+    <t>trf only</t>
+  </si>
+  <si>
+    <t>minke_whale_GCF_000493695.1_BalAcu1.0.trf.0based.sorted.merged.bed</t>
+  </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/reference_genomes/unifiedBedMasksForAllGenomes/vaquita_mPhoSin1</t>
+  </si>
+  <si>
+    <t>vaquita_mPhoSin1.exon10kb.repmask.trf.NEGATIVEMASK.merged.USETHIS.bed</t>
+  </si>
+  <si>
+    <t>repeats only (repmask+trf)</t>
+  </si>
+  <si>
+    <t>vaquita_mPhoSin1.repeatsOnly.repmask.trf.NEGATIVEMASK.merged.bed</t>
+  </si>
+  <si>
+    <t>vaquita_mPhoSin1.exonMask.fromGFF_or_GTF.plusminus10kb.0based.sorted.merged.bed</t>
+  </si>
+  <si>
+    <t>minke_whale_GCF_000493695.1_BalAcu1.0.repeatsOnly.repmask.trf.NEGATIVEMASK.merged.bed</t>
+  </si>
+  <si>
+    <t>mouse_mm10.exonMask.fromGFF_or_GTF.plusminus10kb.0based.sorted.merged.bed</t>
+  </si>
+  <si>
+    <t>mouse_mm10.repeatsOnly.repmask.trf.NEGATIVEMASK.merged.bed</t>
+  </si>
+  <si>
+    <t>mouse_mm10.exon10kb.repmask.trf.NEGATIVEMASK.merged.USETHIS.bed</t>
+  </si>
+  <si>
+    <t>mouse_mm10.trf.0based.sorted.merged.bed</t>
+  </si>
+  <si>
+    <t>mouse_mm10.repeatMasker.0based.sorted.merged.bed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FINAL FILES for records: </t>
+  </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/reference_genomes/unifiedBedMasksForAllGenomes/mouse_mm10</t>
+  </si>
+  <si>
+    <t>humans_GRCh38.repeatsOnly.repmask.trf.NEGATIVEMASK.merged.bed</t>
+  </si>
+  <si>
+    <t>humans_GRCh38.exon10kb.repmask.trf.NEGATIVEMASK.merged.USETHIS.bed</t>
+  </si>
+  <si>
+    <t>humans_GRCh38.trf.0based.sorted.merged.bed</t>
+  </si>
+  <si>
+    <t>humans_GRCh38.repeatMasker.0based.sorted.merged.bed</t>
+  </si>
+  <si>
+    <t>humans_GRCh38.exonMask.fromGFF_or_GTF.plusminus10kb.0based.sorted.merged.bed</t>
+  </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/reference_genomes/unifiedBedMasksForAllGenomes/humans_GRCh38</t>
+  </si>
+  <si>
+    <t>dog_canFam3.exonMask.fromGFF_or_GTF.plusminus10kb.0based.sorted.merged.bed</t>
+  </si>
+  <si>
+    <t>dog_canFam3.repeatsOnly.repmask.trf.NEGATIVEMASK.merged.bed</t>
+  </si>
+  <si>
+    <t>dog_canFam3.exon10kb.repmask.trf.NEGATIVEMASK.merged.USETHIS.bed</t>
+  </si>
+  <si>
+    <t>dog_canFam3.trf.0based.sorted.merged.bed</t>
+  </si>
+  <si>
+    <t>dog_canFam3.repeatMasker.0based.sorted.merged.bed</t>
+  </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/reference_genomes/unifiedBedMasksForAllGenomes/dog_canFam3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -262,8 +371,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="18"/>
+      <name val="Monaco"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FFF2F2F2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -272,6 +392,21 @@
       <i/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -297,11 +432,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,16 +755,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D24E0253-BB8C-EC47-8D26-B37992DB0351}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="9.83203125" customWidth="1"/>
-    <col min="3" max="3" width="31" customWidth="1"/>
+    <col min="3" max="3" width="191" customWidth="1"/>
     <col min="4" max="4" width="32.83203125" customWidth="1"/>
     <col min="5" max="5" width="49" customWidth="1"/>
     <col min="6" max="6" width="49.83203125" customWidth="1"/>
@@ -643,10 +782,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -655,13 +794,13 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -690,7 +829,7 @@
         <v>7</v>
       </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -712,14 +851,14 @@
       <c r="F3" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="H3" t="s">
         <v>10</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -735,7 +874,7 @@
       <c r="D4" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F4" t="s">
@@ -745,27 +884,27 @@
         <v>52</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="E5" t="s">
         <v>63</v>
@@ -777,18 +916,18 @@
         <v>38</v>
       </c>
       <c r="H5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>53</v>
@@ -799,22 +938,22 @@
       <c r="E6" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>32</v>
+      <c r="F6" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
         <v>56</v>
@@ -832,26 +971,235 @@
         <v>60</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>44</v>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98EA5DFC-9EDC-0A4B-9543-9D303C312A23}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
run trf on minke whale as well
</commit_message>
<xml_diff>
--- a/analyses/maskGenomes/pathsToMaskingFiles.xlsx
+++ b/analyses/maskGenomes/pathsToMaskingFiles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annabelbeichman/Documents/UW/DNAShapeProject/scripts/DNA_Shape_Project/analyses/maskGenomes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409C8965-588A-9C46-90BF-B977DE9BD97A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40998BB1-0C58-A243-A006-64AB1D7CD5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="520" windowWidth="36860" windowHeight="20060" activeTab="1" xr2:uid="{69AA28EC-8F56-B44C-B7AC-A26DE8F0EC11}"/>
+    <workbookView xWindow="1600" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{69AA28EC-8F56-B44C-B7AC-A26DE8F0EC11}"/>
   </bookViews>
   <sheets>
     <sheet name="GenomeFiles" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="124">
   <si>
     <t>Species</t>
   </si>
@@ -135,9 +135,6 @@
   </si>
   <si>
     <t>/net/harris/vol1/home/beichman/reference_genomes/homo_sapiens_ancestor_GRCh38/homo_sapiens_ancestor_*.fa</t>
-  </si>
-  <si>
-    <t>RUNNING ON SAGE</t>
   </si>
   <si>
     <t>X</t>
@@ -263,9 +260,6 @@
     <t>minke_whale_GCF_000493695.1_BalAcu1.0.exonMask.fromGFF_or_GTF.plusminus10kb.0based.sorted.merged.bed</t>
   </si>
   <si>
-    <t>rep mask only</t>
-  </si>
-  <si>
     <t>minke_whale_GCF_000493695.1_BalAcu1.0.repeatMasker.0based.sorted.merged.bed</t>
   </si>
   <si>
@@ -348,13 +342,91 @@
   </si>
   <si>
     <t>/net/harris/vol1/home/beichman/reference_genomes/unifiedBedMasksForAllGenomes/dog_canFam3</t>
+  </si>
+  <si>
+    <t>snp file notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excludes repeat/trf regions already. Cpg islands are present. Dense snp regions excluded. </t>
+  </si>
+  <si>
+    <t>sample notes</t>
+  </si>
+  <si>
+    <t>need to exclude relatives</t>
+  </si>
+  <si>
+    <t>polarization notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">was polarized by JAR </t>
+  </si>
+  <si>
+    <t>Apes</t>
+  </si>
+  <si>
+    <t>Should think about not including multiple pops if we aren't doing hamming distance?? Keep them in processing just in case</t>
+  </si>
+  <si>
+    <t>need to figure out solution to shared variation and ksfs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">need to run spectrm </t>
+  </si>
+  <si>
+    <t>ENP ksfs seems kind of weird compared to GOC after polarization -- not sure what that's about.</t>
+  </si>
+  <si>
+    <t>don't get too worried about polarization because we are going to also show that folded spectra show signal</t>
+  </si>
+  <si>
+    <t>whole genome, but cpg islands removed (by me?) -- maybe refilter and keep in CpG islands if possible? Look into filtering more</t>
+  </si>
+  <si>
+    <t>all sites</t>
+  </si>
+  <si>
+    <t>callability mask based on coverage</t>
+  </si>
+  <si>
+    <t>all sites; could use callability mask</t>
+  </si>
+  <si>
+    <t>issue: some sort of coverage map? Possible for minke, vaquita, brown bear, apes. Human callability mask. But mouse??!?!</t>
+  </si>
+  <si>
+    <t>Instead lets just mask all these repeat regions and call it fine.</t>
+  </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/reference_genomes/brown_bear/trf/trf.output.sorted.merged.0based.bed</t>
+  </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/reference_genomes/unifiedBedMasksForAllGenomes/brown_bear_GCF_003584765.1</t>
+  </si>
+  <si>
+    <t>brown_bear_GCF_003584765.1.repeatsOnly.repmask.trf.NEGATIVEMASK.merged.bed</t>
+  </si>
+  <si>
+    <t>brown_bear_GCF_003584765.1.exon10kb.repmask.trf.NEGATIVEMASK.merged.USETHIS.bed</t>
+  </si>
+  <si>
+    <t>repeat masker only</t>
+  </si>
+  <si>
+    <t>brown_bear_GCF_003584765.1.trf.0based.sorted.merged.bed</t>
+  </si>
+  <si>
+    <t>brown_bear_GCF_003584765.1.repeatMasker.0based.sorted.merged.bed</t>
+  </si>
+  <si>
+    <t>brown_bear_GCF_003584765.1.exonMask.fromGFF_or_GTF.plusminus10kb.0based.sorted.merged.bed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -371,19 +443,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="18"/>
-      <name val="Monaco"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FFF2F2F2"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -432,15 +493,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -757,14 +816,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D24E0253-BB8C-EC47-8D26-B37992DB0351}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="9.83203125" customWidth="1"/>
-    <col min="3" max="3" width="191" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" customWidth="1"/>
     <col min="4" max="4" width="32.83203125" customWidth="1"/>
     <col min="5" max="5" width="49" customWidth="1"/>
     <col min="6" max="6" width="49.83203125" customWidth="1"/>
@@ -794,7 +853,7 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I1" t="s">
         <v>24</v>
@@ -811,19 +870,19 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
         <v>39</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>40</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>41</v>
       </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2" t="s">
         <v>7</v>
@@ -840,18 +899,18 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
         <v>46</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>47</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>48</v>
       </c>
-      <c r="F3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" t="s">
@@ -869,22 +928,22 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" t="s">
         <v>51</v>
       </c>
-      <c r="F4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" t="s">
-        <v>52</v>
-      </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I4" t="s">
         <v>27</v>
@@ -900,23 +959,23 @@
       <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>64</v>
+      <c r="D5" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" t="s">
         <v>37</v>
       </c>
-      <c r="G5" t="s">
-        <v>38</v>
-      </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" t="s">
         <v>28</v>
@@ -930,22 +989,22 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" t="s">
         <v>53</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>54</v>
       </c>
-      <c r="E6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G6" s="4" t="s">
+      <c r="F6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H6" t="s">
         <v>33</v>
-      </c>
-      <c r="H6" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -956,46 +1015,54 @@
         <v>22</v>
       </c>
       <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
         <v>56</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>57</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>58</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>59</v>
       </c>
-      <c r="G7" t="s">
-        <v>60</v>
-      </c>
       <c r="H7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>36</v>
+      <c r="H8" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D11" s="6" t="s">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>44</v>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -1006,144 +1073,161 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" t="s">
+        <v>120</v>
+      </c>
+      <c r="G16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" t="s">
         <v>67</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" t="s">
         <v>77</v>
       </c>
-      <c r="E16" t="s">
-        <v>69</v>
-      </c>
-      <c r="F16" t="s">
-        <v>71</v>
-      </c>
-      <c r="G16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="F18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="E19" t="s">
         <v>79</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="F19" t="s">
+        <v>83</v>
+      </c>
+      <c r="G19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="G20" t="s">
         <v>88</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+      <c r="B21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" t="s">
+        <v>119</v>
+      </c>
+      <c r="D21" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" t="s">
+        <v>123</v>
+      </c>
+      <c r="F21" t="s">
+        <v>122</v>
+      </c>
+      <c r="G21" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="B22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" t="s">
         <v>96</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="G22" t="s">
         <v>95</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1154,52 +1238,120 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98EA5DFC-9EDC-0A4B-9543-9D303C312A23}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="46.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="B7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding script to find cpg windows (ala ucsc) for brown bear
</commit_message>
<xml_diff>
--- a/analyses/maskGenomes/pathsToMaskingFiles.xlsx
+++ b/analyses/maskGenomes/pathsToMaskingFiles.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annabelbeichman/Documents/UW/DNAShapeProject/scripts/DNA_Shape_Project/analyses/maskGenomes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40998BB1-0C58-A243-A006-64AB1D7CD5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4520B645-C22D-D04F-9B49-3F3A7CB21603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1600" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{69AA28EC-8F56-B44C-B7AC-A26DE8F0EC11}"/>
   </bookViews>
   <sheets>
     <sheet name="GenomeFiles" sheetId="1" r:id="rId1"/>
     <sheet name="PreprocessingNotes" sheetId="2" r:id="rId2"/>
+    <sheet name="NotesOnRunningMutyper" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="159">
   <si>
     <t>Species</t>
   </si>
@@ -59,18 +60,12 @@
     <t>/net/harris/vol1/home/beichman/reference_genomes/minke_whale/minke_whale_genome/GCF_000493695.1_BalAcu1.0</t>
   </si>
   <si>
-    <t>CpG_repeats.bed</t>
-  </si>
-  <si>
     <t>Vaquita</t>
   </si>
   <si>
     <t>/net/harris/vol1/home/beichman/reference_genomes/vaquita/mPhoSin1.pri.cur.20190723_rename</t>
   </si>
   <si>
-    <t>mPhoSin1.pri.cur.20190723_rename_cpgIslands.bed </t>
-  </si>
-  <si>
     <t>COMBINED WITH RM output</t>
   </si>
   <si>
@@ -110,15 +105,15 @@
     <t>GFF_or_GTF_path</t>
   </si>
   <si>
+    <t xml:space="preserve">NEED TO RUN </t>
+  </si>
+  <si>
     <t>SNPFileNote</t>
   </si>
   <si>
     <t>repeats filtered out by JAR, but CpG islands still present</t>
   </si>
   <si>
-    <t>check if I have whole genome files (I think I do)</t>
-  </si>
-  <si>
     <t>no regional filtering</t>
   </si>
   <si>
@@ -137,39 +132,15 @@
     <t>/net/harris/vol1/home/beichman/reference_genomes/homo_sapiens_ancestor_GRCh38/homo_sapiens_ancestor_*.fa</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>CpGIslands -- not going to use</t>
-  </si>
-  <si>
     <t>not using ^^</t>
   </si>
   <si>
     <t>/net/harris/vol1/home/beichman/reference_genomes/human_GRCh38_annotation/repeatmask.sorted.bed</t>
   </si>
   <si>
-    <r>
-      <t>/net/harris/vol1/home/beichman/reference_genomes/human_GRCh38_annotation/hg38.trf.bed.gz</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFF2F2F2"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
     <t>/net/harris/vol1/home/beichman/reference_genomes/minke_whale/minke_whale_genome/GCF_000493695.1_BalAcu1.0/BalAcu1.0.fa</t>
   </si>
   <si>
-    <t>/net/harris/vol1/home/beichman/reference_genomes/minke_whale/minke_whale_genome/GCF_000493695.1_BalAcu1.0/BalAcu1.0.fa.fai    </t>
-  </si>
-  <si>
     <t>/net/harris/vol1/home/beichman/reference_genomes/minke_whale/minke_whale_genome/GCF_000493695.1_BalAcu1.0/GCF_000493695.1_BalAcu1.0_genomic.gff.gz</t>
   </si>
   <si>
@@ -182,12 +153,6 @@
     <t>/net/harris/vol1/home/beichman/unifiedBedMasksForAllGenomes</t>
   </si>
   <si>
-    <t>/net/harris/vol1/home/beichman/reference_genomes/minke_whale/minke_whale_genome/GCF_000493695.1_BalAcu1.0/AnnabelDownloads_notusedbyMeixi/balAcu1.trf.bed.gz</t>
-  </si>
-  <si>
-    <t>/net/harris/vol1/home/beichman/reference_genomes/vaquita/mPhoSin1.pri.cur.20190723_rename/mPhoSin1.pri.cur.20190723_rename.fasta   </t>
-  </si>
-  <si>
     <t>/net/harris/vol1/home/beichman/reference_genomes/vaquita/mPhoSin1.pri.cur.20190723_rename/mPhoSin1.pri.cur.20190723_rename.fasta.fai</t>
   </si>
   <si>
@@ -206,24 +171,12 @@
     <t>/net/harris/vol1/home/beichman/reference_genomes/mouse/mm10_aka_mm38/REPEATS/trfMaskChrom/mm10.trf.chr1-19_ONLY.ABcombined.bed</t>
   </si>
   <si>
-    <t>/net/harris/vol1/home/beichman/reference_genomes/brown_bear/brown_bear.fasta </t>
-  </si>
-  <si>
-    <t> /net/harris/vol1/home/beichman/reference_genomes/brown_bear/brown_bear.fasta.fai  </t>
-  </si>
-  <si>
     <t>/net/harris/vol1/home/beichman/reference_genomes/brown_bear/GCF_003584765.1_ASM358476v1_genomic.gff.gz</t>
   </si>
   <si>
     <t>/net/harris/vol1/home/beichman/reference_genomes/canFam3/canFam3.fa</t>
   </si>
   <si>
-    <t>/net/harris/vol1/home/beichman/reference_genomes/canFam3/ canFam3.fa.fai </t>
-  </si>
-  <si>
-    <t xml:space="preserve">/net/harris/vol1/home/beichman/reference_genomes/canFam3/annotation/canFam3.ensGene.gtf.gz </t>
-  </si>
-  <si>
     <t>/net/harris/vol1/home/beichman/reference_genomes/canFam3/canFam3.fa.RepeatMasker.sorted.bed</t>
   </si>
   <si>
@@ -347,9 +300,6 @@
     <t>snp file notes</t>
   </si>
   <si>
-    <t xml:space="preserve">excludes repeat/trf regions already. Cpg islands are present. Dense snp regions excluded. </t>
-  </si>
-  <si>
     <t>sample notes</t>
   </si>
   <si>
@@ -386,9 +336,6 @@
     <t>all sites</t>
   </si>
   <si>
-    <t>callability mask based on coverage</t>
-  </si>
-  <si>
     <t>all sites; could use callability mask</t>
   </si>
   <si>
@@ -420,13 +367,160 @@
   </si>
   <si>
     <t>brown_bear_GCF_003584765.1.exonMask.fromGFF_or_GTF.plusminus10kb.0based.sorted.merged.bed</t>
+  </si>
+  <si>
+    <t>callability mask based on coverage - should I not use?</t>
+  </si>
+  <si>
+    <t>excludes repeat/trf regions already. Cpg islands are present. Dense snp regions excluded. Has ANN= annotation of ancestral alleles</t>
+  </si>
+  <si>
+    <t>Note: need to use polarized vcfs and ancestral fastas</t>
+  </si>
+  <si>
+    <t>polarized vcfs because sites that couldn't be polarized were removed (except for humans were you use --strict because sites that couldn’t be polarized are soft masked in anc fasta)</t>
+  </si>
+  <si>
+    <t>Want to make notes on what I should use and what was actually used to make sure everything is legit</t>
+  </si>
+  <si>
+    <t>vaquita</t>
+  </si>
+  <si>
+    <t>Note : vcf files should include sites with ancestral alleles; any site that couldn't be polarized should be excluded</t>
+  </si>
+  <si>
+    <t>Should I redo polarization?</t>
+  </si>
+  <si>
+    <t>vcf that was used</t>
+  </si>
+  <si>
+    <t>is that the vcf that should be used?</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/vaquita/vcfs/SNPsOnly/polarized/20210216/vaquita_20_simple_PASS_autos_variants_outgroupAlleles_ancAllele.vcf.gz</t>
+  </si>
+  <si>
+    <t>script</t>
+  </si>
+  <si>
+    <t>/Users/annabelbeichman/Documents/UW/WhaleProject/vaquita/VaquitaSpectrum/analyses/mutyper/RunMutyperOnSage.SeparatesByPopulationVaquita.7merContext.sh</t>
+  </si>
+  <si>
+    <t>individuals to exclude</t>
+  </si>
+  <si>
+    <t>z0001663, z0004380, z0004393, z0004394, z0185383</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>resulting variants file</t>
+  </si>
+  <si>
+    <t>included --strict but that's ok bc vaquita has no softmasking; repeat regions and trf regions already excluded from SNP file</t>
+  </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/vaquita/analyses/mutyper/mutyperResults_20210225_7mer/mutyper_variant_files/allInds.exceptRelatives.mutyper.variants.mutationTypes.noFixedSites.AncestralDerivedNotRefAlt.SomeRevComped.Strict.7mer.ALLFREQS.vcf.gz</t>
+  </si>
+  <si>
+    <t>minke whale</t>
+  </si>
+  <si>
+    <t>/Users/annabelbeichman/Documents/UW/WhaleProject/fin_whales/fin_whale_scripts/fin_whale_spectrum/analyses/mutyper/whole_genome_KeightleyPolarized/runMutyper.OnFinWhales.7mer.NOSTRICT.WholeGenome.PASSSitesOnly.KeightleyPolarized.sh</t>
+  </si>
+  <si>
+    <t>BalAcu02,BalMus01,MegNov01,EubGla01,ENPOR12,ENPAK28</t>
+  </si>
+  <si>
+    <t>has CpG islands masked - need to deal with that</t>
+  </si>
+  <si>
+    <t xml:space="preserve">only sites with high confidence polarization were included - this maybe skewed ENP ksfs more than GOC </t>
+  </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/reference_genomes/mouse/mm10_aka_mm38/CpGIslands_fromUCSC/mm10.CpGIslandsTrack.UCSC.bed.gz</t>
+  </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/reference_genomes/human_GRCh38_annotation/humanGRCh38.CpGIslandsTrack.UCSC.bed.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISSUE: minke whale from ucsc uses different coordinates that ncbi. Do any others have that issue? </t>
+  </si>
+  <si>
+    <t>are coordinates ok between all files?</t>
+  </si>
+  <si>
+    <t>yes whole genomes, but Cpg Islands and repeats were masked already</t>
+  </si>
+  <si>
+    <t>whole genoems</t>
+  </si>
+  <si>
+    <t>whole genomes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ok for fin whale what I think I want to do is : reannotate vcf with ancestral alleles removing fail sites, but keeping warn_CpGRep(???) anything; have to update ancestral fasta again too -- boo; then </t>
+  </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/reference_genomes/minke_whale/minke_whale_genome/GCF_000493695.1_BalAcu1.0/ucsc/CpG_ExtUnmasked.bed</t>
+  </si>
+  <si>
+    <t>note that meixi et al converted cpg islands coords from ucsc to refseq</t>
+  </si>
+  <si>
+    <t>UPDATE THE SCRIPT WITH THESE NEW FILES!!!!</t>
+  </si>
+  <si>
+    <t>CpG Islands</t>
+  </si>
+  <si>
+    <t>** IF ADDING ANY NEW SPECIES, MAKE SURE COORDINATES ACROSS FILES ARE THE SAME -- CAN BE AN ISSUE WITH UCSC AND REFSEQ ***</t>
+  </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/reference_genomes/canFam3/canFam3.CpGIslandsTrack.UCSC.bed.gz</t>
+  </si>
+  <si>
+    <t>running on sage on 20220401</t>
+  </si>
+  <si>
+    <t>need to update the script to have cpg islands incorporated</t>
+  </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/reference_genomes/brown_bear/brown_bear.fasta</t>
+  </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/reference_genomes/vaquita/mPhoSin1.pri.cur.20190723_rename/mPhoSin1.pri.cur.20190723_rename.fasta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/net/harris/vol1/home/beichman/reference_genomes/minke_whale/minke_whale_genome/GCF_000493695.1_BalAcu1.0/BalAcu1.0.fa.fai </t>
+  </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/reference_genomes/brown_bear/brown_bear.fasta.fai</t>
+  </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/reference_genomes/canFam3/ canFam3.fa.fai</t>
+  </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/reference_genomes/canFam3/annotation/canFam3.ensGene.gtf.gz</t>
+  </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/reference_genomes/human_GRCh38_annotation/hg38.trf.bed.gz</t>
+  </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/reference_genomes/vaquita/mPhoSin1.pri.cur.20190723_rename/mPhoSin1.pri.cur.20190723_rename_cpgIslands.bed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -435,16 +529,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
-      <color rgb="FFF2F2F2"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -472,6 +566,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -493,13 +595,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -814,421 +924,470 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D24E0253-BB8C-EC47-8D26-B37992DB0351}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="9.83203125" customWidth="1"/>
-    <col min="3" max="3" width="33.6640625" customWidth="1"/>
-    <col min="4" max="4" width="32.83203125" customWidth="1"/>
-    <col min="5" max="5" width="49" customWidth="1"/>
-    <col min="6" max="6" width="49.83203125" customWidth="1"/>
-    <col min="7" max="7" width="116.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H3" t="s">
+        <v>143</v>
+      </c>
+      <c r="I3" t="s">
+        <v>139</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="L3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>158</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" t="s">
+        <v>120</v>
+      </c>
+      <c r="L4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" t="s">
+        <v>135</v>
+      </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="D6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
+        <v>157</v>
+      </c>
+      <c r="H6" t="s">
+        <v>136</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" t="s">
+        <v>102</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
         <v>45</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D8" t="s">
+        <v>155</v>
+      </c>
+      <c r="E8" t="s">
+        <v>156</v>
+      </c>
+      <c r="F8" t="s">
         <v>46</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G8" t="s">
         <v>47</v>
       </c>
-      <c r="F3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="H8" t="s">
+        <v>148</v>
+      </c>
+      <c r="I8" t="s">
+        <v>140</v>
+      </c>
+      <c r="K8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J4" t="s">
+      <c r="H9" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G5" t="s">
+      <c r="E12" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G6" t="s">
-        <v>116</v>
-      </c>
-      <c r="H6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G7" t="s">
-        <v>59</v>
-      </c>
-      <c r="H7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J14" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" t="s">
-        <v>75</v>
-      </c>
-      <c r="E16" t="s">
-        <v>68</v>
-      </c>
-      <c r="F16" t="s">
-        <v>120</v>
-      </c>
-      <c r="G16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" t="s">
-        <v>67</v>
+        <v>5</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="E17" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="G17" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18" t="s">
-        <v>74</v>
+        <v>53</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E18" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="F18" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="G18" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" t="s">
         <v>12</v>
       </c>
-      <c r="B19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" t="s">
-        <v>79</v>
-      </c>
-      <c r="F19" t="s">
-        <v>83</v>
-      </c>
       <c r="G19" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>91</v>
-      </c>
-      <c r="C20" t="s">
-        <v>87</v>
+        <v>73</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="D20" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="E20" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="F20" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="G20" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21" t="s">
-        <v>119</v>
+        <v>79</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="D21" t="s">
-        <v>118</v>
+        <v>74</v>
       </c>
       <c r="E21" t="s">
-        <v>123</v>
+        <v>78</v>
       </c>
       <c r="F21" t="s">
-        <v>122</v>
+        <v>77</v>
       </c>
       <c r="G21" t="s">
-        <v>121</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" t="s">
-        <v>94</v>
+        <v>103</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="D22" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="E22" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="F22" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="G22" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>18</v>
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" t="s">
+        <v>80</v>
+      </c>
+      <c r="F23" t="s">
+        <v>84</v>
+      </c>
+      <c r="G23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1238,10 +1397,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98EA5DFC-9EDC-0A4B-9543-9D303C312A23}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1255,13 +1414,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C1" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1269,89 +1428,189 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>18</v>
+      <c r="A8" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="B9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>109</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1CBEA7-77F1-F841-B5F2-CB2E5FBC1069}">
+  <dimension ref="A2:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="7" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="B6" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E8" t="s">
+        <v>132</v>
+      </c>
+      <c r="F8" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating vaquita config file
</commit_message>
<xml_diff>
--- a/analyses/maskGenomes/pathsToMaskingFiles.xlsx
+++ b/analyses/maskGenomes/pathsToMaskingFiles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annabelbeichman/Documents/UW/DNAShapeProject/scripts/DNA_Shape_Project/analyses/maskGenomes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4520B645-C22D-D04F-9B49-3F3A7CB21603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C486A2-54A5-5C47-AB14-275E87792C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{69AA28EC-8F56-B44C-B7AC-A26DE8F0EC11}"/>
+    <workbookView xWindow="1600" yWindow="500" windowWidth="28800" windowHeight="16500" activeTab="1" xr2:uid="{69AA28EC-8F56-B44C-B7AC-A26DE8F0EC11}"/>
   </bookViews>
   <sheets>
     <sheet name="GenomeFiles" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="176">
   <si>
     <t>Species</t>
   </si>
@@ -105,9 +105,6 @@
     <t>GFF_or_GTF_path</t>
   </si>
   <si>
-    <t xml:space="preserve">NEED TO RUN </t>
-  </si>
-  <si>
     <t>SNPFileNote</t>
   </si>
   <si>
@@ -132,9 +129,6 @@
     <t>/net/harris/vol1/home/beichman/reference_genomes/homo_sapiens_ancestor_GRCh38/homo_sapiens_ancestor_*.fa</t>
   </si>
   <si>
-    <t>not using ^^</t>
-  </si>
-  <si>
     <t>/net/harris/vol1/home/beichman/reference_genomes/human_GRCh38_annotation/repeatmask.sorted.bed</t>
   </si>
   <si>
@@ -201,12 +195,6 @@
     <t>/net/harris/vol1/home/beichman/reference_genomes/unifiedBedMasksForAllGenomes/minke_whale_GCF_000493695.1_BalAcu1.0</t>
   </si>
   <si>
-    <t>exon10kb+repmask+trf unified bed USE THIS</t>
-  </si>
-  <si>
-    <t>minke_whale_GCF_000493695.1_BalAcu1.0.exon10kb.repmask.trf.NEGATIVEMASK.merged.USETHIS.bed</t>
-  </si>
-  <si>
     <t>exon10kb only</t>
   </si>
   <si>
@@ -225,9 +213,6 @@
     <t>/net/harris/vol1/home/beichman/reference_genomes/unifiedBedMasksForAllGenomes/vaquita_mPhoSin1</t>
   </si>
   <si>
-    <t>vaquita_mPhoSin1.exon10kb.repmask.trf.NEGATIVEMASK.merged.USETHIS.bed</t>
-  </si>
-  <si>
     <t>repeats only (repmask+trf)</t>
   </si>
   <si>
@@ -246,9 +231,6 @@
     <t>mouse_mm10.repeatsOnly.repmask.trf.NEGATIVEMASK.merged.bed</t>
   </si>
   <si>
-    <t>mouse_mm10.exon10kb.repmask.trf.NEGATIVEMASK.merged.USETHIS.bed</t>
-  </si>
-  <si>
     <t>mouse_mm10.trf.0based.sorted.merged.bed</t>
   </si>
   <si>
@@ -264,9 +246,6 @@
     <t>humans_GRCh38.repeatsOnly.repmask.trf.NEGATIVEMASK.merged.bed</t>
   </si>
   <si>
-    <t>humans_GRCh38.exon10kb.repmask.trf.NEGATIVEMASK.merged.USETHIS.bed</t>
-  </si>
-  <si>
     <t>humans_GRCh38.trf.0based.sorted.merged.bed</t>
   </si>
   <si>
@@ -285,9 +264,6 @@
     <t>dog_canFam3.repeatsOnly.repmask.trf.NEGATIVEMASK.merged.bed</t>
   </si>
   <si>
-    <t>dog_canFam3.exon10kb.repmask.trf.NEGATIVEMASK.merged.USETHIS.bed</t>
-  </si>
-  <si>
     <t>dog_canFam3.trf.0based.sorted.merged.bed</t>
   </si>
   <si>
@@ -354,9 +330,6 @@
     <t>brown_bear_GCF_003584765.1.repeatsOnly.repmask.trf.NEGATIVEMASK.merged.bed</t>
   </si>
   <si>
-    <t>brown_bear_GCF_003584765.1.exon10kb.repmask.trf.NEGATIVEMASK.merged.USETHIS.bed</t>
-  </si>
-  <si>
     <t>repeat masker only</t>
   </si>
   <si>
@@ -474,9 +447,6 @@
     <t>note that meixi et al converted cpg islands coords from ucsc to refseq</t>
   </si>
   <si>
-    <t>UPDATE THE SCRIPT WITH THESE NEW FILES!!!!</t>
-  </si>
-  <si>
     <t>CpG Islands</t>
   </si>
   <si>
@@ -486,9 +456,6 @@
     <t>/net/harris/vol1/home/beichman/reference_genomes/canFam3/canFam3.CpGIslandsTrack.UCSC.bed.gz</t>
   </si>
   <si>
-    <t>running on sage on 20220401</t>
-  </si>
-  <si>
     <t>need to update the script to have cpg islands incorporated</t>
   </si>
   <si>
@@ -514,23 +481,100 @@
   </si>
   <si>
     <t>/net/harris/vol1/home/beichman/reference_genomes/vaquita/mPhoSin1.pri.cur.20190723_rename/mPhoSin1.pri.cur.20190723_rename_cpgIslands.bed</t>
+  </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/reference_genomes/brown_bear/CpGIslands.fromcpgplot.emboss.output.bed</t>
+  </si>
+  <si>
+    <t>/net/harris/vol1/home/beichman/reference_genomes/minke_whale/minke_whale_genome/GCF_000493695.1_BalAcu1.0/trf/trf.output.sorted.merged.0based.bed</t>
+  </si>
+  <si>
+    <t>exon10kb+repmask+trf unified bed BUT NO CPG ISLANDS</t>
+  </si>
+  <si>
+    <t>minke_whale_GCF_000493695.1_BalAcu1.0.exon10kb.repmask.trf.NEGATIVEMASK.merged.bed</t>
+  </si>
+  <si>
+    <t>vaquita_mPhoSin1.exon10kb.repmask.trf.NEGATIVEMASK.merged.bed</t>
+  </si>
+  <si>
+    <t>mouse_mm10.exon10kb.repmask.trf.NEGATIVEMASK.merged.bed</t>
+  </si>
+  <si>
+    <t>humans_GRCh38.exon10kb.repmask.trf.NEGATIVEMASK.merged.bed</t>
+  </si>
+  <si>
+    <t>brown_bear_GCF_003584765.1.exon10kb.repmask.trf.NEGATIVEMASK.merged.bed</t>
+  </si>
+  <si>
+    <t>dog_canFam3.exon10kb.repmask.trf.NEGATIVEMASK.merged.bed</t>
+  </si>
+  <si>
+    <t>ALL THE THINGS : exon10kb+repmask+trf+cpgislands</t>
+  </si>
+  <si>
+    <t>minke_whale_GCF_000493695.1_BalAcu1.0.exon10kb.repmask.trf.cpgIslands.NEGATIVEMASK.merged.USETHIS.bed</t>
+  </si>
+  <si>
+    <t>vaquita_mPhoSin1.exon10kb.repmask.trf.cpgIslands.NEGATIVEMASK.merged.USETHIS.bed</t>
+  </si>
+  <si>
+    <t>dog_canFam3.exon10kb.repmask.trf.cpgIslands.NEGATIVEMASK.merged.USETHIS.bed</t>
+  </si>
+  <si>
+    <t>mouse_mm10.exon10kb.repmask.trf.cpgIslands.NEGATIVEMASK.merged.USETHIS.bed</t>
+  </si>
+  <si>
+    <t>humans_GRCh38.exon10kb.repmask.trf.cpgIslands.NEGATIVEMASK.merged.USETHIS.bed</t>
+  </si>
+  <si>
+    <t>brown_bear_GCF_003584765.1.exon10kb.repmask.trf.cpgIslands.NEGATIVEMASK.merged.USETHIS.bed</t>
+  </si>
+  <si>
+    <t>UPDATED THE SCRIPT WITH THESE NEW FILES!!!!</t>
+  </si>
+  <si>
+    <t>filters prior to mutyper variants</t>
+  </si>
+  <si>
+    <t>/Users/annabelbeichman/Documents/UW/DNAShapeProject/scripts/DNA_Shape_Project/analyses/mutyper/apes/runMutyper.AnyVCFREF.NOSTRICT.apes.sh</t>
+  </si>
+  <si>
+    <t>excluding relatives; repeats were already excluded; cpg islands were included</t>
+  </si>
+  <si>
+    <t>PASS; m2 M2; -v snp; missing data sites removed</t>
+  </si>
+  <si>
+    <t>/Users/annabelbeichman/Documents/UW/WhaleProject/vaquita/VaquitaSpectrum/analyses/mutyper/humans/runMutyper.AnyVCFREF.STRICT.Humans.sh</t>
+  </si>
+  <si>
+    <t>none (good to go)</t>
+  </si>
+  <si>
+    <t>not done yet</t>
+  </si>
+  <si>
+    <t>/Users/annabelbeichman/Documents/UW/BearProject/scripts/BearAdmixtureProject/analyses/mutyper/RunMutyperOnSage.SeparatesByPopulation.bears.7mer.NOSTRICT.sh</t>
+  </si>
+  <si>
+    <t>masked repeats</t>
+  </si>
+  <si>
+    <t>need to redo</t>
+  </si>
+  <si>
+    <t>/Users/annabelbeichman/Documents/UW/BearProject/scripts/BearAdmixtureProject/analyses/mutyper/runMutyper.7mer.MICE.PerChromosome.KeightleyPolarization.NOSTRICT.REPEATMASK.sh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -566,14 +610,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -595,21 +631,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -926,14 +960,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D24E0253-BB8C-EC47-8D26-B37992DB0351}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="9.83203125" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="7.83203125" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" customWidth="1"/>
     <col min="6" max="6" width="23.1640625" customWidth="1"/>
@@ -942,43 +976,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="H2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>138</v>
+      <c r="K2" s="2" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -989,31 +1023,31 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
         <v>33</v>
       </c>
-      <c r="D3" t="s">
-        <v>153</v>
-      </c>
-      <c r="E3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="3" t="s">
         <v>149</v>
       </c>
       <c r="H3" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="I3" t="s">
-        <v>139</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>144</v>
+        <v>130</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="L3" t="s">
-        <v>145</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1024,31 +1058,31 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
         <v>38</v>
       </c>
-      <c r="E4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="I4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K4" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="L4" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -1059,31 +1093,31 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" t="s">
         <v>41</v>
       </c>
-      <c r="D5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" t="s">
-        <v>43</v>
-      </c>
       <c r="H5" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="I5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K5" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1093,29 +1127,29 @@
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" t="s">
-        <v>32</v>
-      </c>
       <c r="G6" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="H6" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="I6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K6" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1126,28 +1160,28 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="D7" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>52</v>
+        <v>42</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="G7" t="s">
-        <v>102</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>22</v>
+        <v>94</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>148</v>
       </c>
       <c r="I7" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="K7" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -1158,235 +1192,253 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" t="s">
+        <v>145</v>
+      </c>
+      <c r="F8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" t="s">
         <v>45</v>
       </c>
-      <c r="D8" t="s">
-        <v>155</v>
-      </c>
-      <c r="E8" t="s">
-        <v>156</v>
-      </c>
-      <c r="F8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" t="s">
-        <v>47</v>
-      </c>
       <c r="H8" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="I8" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="K8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>31</v>
+      <c r="B9" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>137</v>
+      <c r="A10" s="2" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>100</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>37</v>
+        <v>92</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="J14" s="3" t="s">
-        <v>142</v>
+      <c r="J14" s="2" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>0</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" t="s">
-        <v>63</v>
+      <c r="C17" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="E17" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F17" t="s">
-        <v>106</v>
+        <v>52</v>
       </c>
       <c r="G17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="H17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
       <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>158</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" t="s">
-        <v>57</v>
-      </c>
-      <c r="F18" t="s">
-        <v>58</v>
-      </c>
       <c r="G18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+      <c r="H18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" t="s">
-        <v>64</v>
+        <v>57</v>
+      </c>
+      <c r="C19" t="s">
+        <v>159</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F19" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="G19" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="C20" t="s">
+        <v>161</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="E20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F20" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="G20" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="H20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+      <c r="C21" t="s">
+        <v>162</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>154</v>
       </c>
       <c r="E21" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="F21" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G21" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="H21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D22" t="s">
-        <v>104</v>
+        <v>95</v>
+      </c>
+      <c r="C22" t="s">
+        <v>163</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>155</v>
       </c>
       <c r="E22" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="F22" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="G22" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+      <c r="H22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" t="s">
-        <v>81</v>
+        <v>77</v>
+      </c>
+      <c r="C23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>156</v>
       </c>
       <c r="E23" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F23" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="G23" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1397,10 +1449,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98EA5DFC-9EDC-0A4B-9543-9D303C312A23}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1409,118 +1461,157 @@
     <col min="2" max="2" width="46.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+      <c r="E1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="E2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+      <c r="E3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="E4" t="s">
+        <v>173</v>
+      </c>
+      <c r="F4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+      <c r="E5" t="s">
+        <v>168</v>
+      </c>
+      <c r="F5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="E6" t="s">
+        <v>170</v>
+      </c>
+      <c r="F6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="E9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1540,77 +1631,77 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="6" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="B6" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" s="7" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C6" s="7" t="s">
+    </row>
+    <row r="7" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="C7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>120</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C8" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D8" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E8" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="F8" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>